<commit_message>
Bug Fixes in - Tax Ledgers Master page Group Masters page print pdf page
</commit_message>
<xml_diff>
--- a/MWBTCustomerCreation/CCAPortal/Docs/itemExcelFile.xlsx
+++ b/MWBTCustomerCreation/CCAPortal/Docs/itemExcelFile.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AF$3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="53">
   <si>
     <t>TallyItemName</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>ItemName</t>
+  </si>
+  <si>
+    <t>Rate</t>
   </si>
   <si>
     <t>Alias</t>
@@ -180,10 +183,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="&quot;&quot;0"/>
   </numFmts>
   <fonts count="22">
@@ -208,14 +211,58 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -224,48 +271,34 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -277,76 +310,46 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -391,13 +394,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.0999786370433668"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.0999786370433668"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -409,175 +568,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -613,16 +616,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -638,30 +641,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,6 +680,30 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -712,148 +715,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="35" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -865,15 +868,15 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -889,13 +892,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -903,6 +903,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1235,48 +1238,48 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:AF3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AE1" sqref="AE1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="47.1428571428571" customWidth="1"/>
     <col min="2" max="2" width="31.2857142857143" customWidth="1"/>
-    <col min="3" max="3" width="33.8571428571429" customWidth="1"/>
-    <col min="4" max="4" width="13.1428571428571" customWidth="1"/>
-    <col min="5" max="5" width="25.2857142857143" customWidth="1"/>
-    <col min="6" max="6" width="25.7142857142857" customWidth="1"/>
-    <col min="7" max="7" width="12.2857142857143" customWidth="1"/>
-    <col min="8" max="8" width="11.4285714285714" customWidth="1"/>
-    <col min="9" max="9" width="25" customWidth="1"/>
-    <col min="10" max="10" width="24.1428571428571" customWidth="1"/>
-    <col min="11" max="11" width="17.8571428571429" customWidth="1"/>
-    <col min="12" max="12" width="16.1428571428571" customWidth="1"/>
-    <col min="13" max="13" width="16.8571428571429" customWidth="1"/>
-    <col min="14" max="14" width="11.5714285714286" customWidth="1"/>
-    <col min="15" max="15" width="11.7142857142857" customWidth="1"/>
-    <col min="16" max="16" width="19.5714285714286" customWidth="1"/>
-    <col min="17" max="17" width="13.1428571428571" customWidth="1"/>
-    <col min="18" max="18" width="23.2857142857143" customWidth="1"/>
-    <col min="19" max="19" width="17" customWidth="1"/>
-    <col min="20" max="20" width="7.71428571428571" customWidth="1"/>
-    <col min="21" max="21" width="22.4285714285714" customWidth="1"/>
-    <col min="22" max="22" width="16.2857142857143" customWidth="1"/>
-    <col min="23" max="23" width="31.1428571428571" customWidth="1"/>
-    <col min="24" max="24" width="18.5714285714286" customWidth="1"/>
-    <col min="25" max="25" width="17.7142857142857" customWidth="1"/>
-    <col min="26" max="26" width="17.4285714285714" customWidth="1"/>
-    <col min="27" max="27" width="21.7142857142857" customWidth="1"/>
-    <col min="28" max="28" width="13.2857142857143" customWidth="1"/>
-    <col min="29" max="29" width="75" customWidth="1"/>
-    <col min="30" max="30" width="9.28571428571429" customWidth="1"/>
-    <col min="31" max="31" width="24.7142857142857" customWidth="1"/>
+    <col min="3" max="4" width="33.8571428571429" customWidth="1"/>
+    <col min="5" max="5" width="13.1428571428571" customWidth="1"/>
+    <col min="6" max="6" width="25.2857142857143" customWidth="1"/>
+    <col min="7" max="7" width="25.7142857142857" customWidth="1"/>
+    <col min="8" max="8" width="12.2857142857143" customWidth="1"/>
+    <col min="9" max="9" width="11.4285714285714" customWidth="1"/>
+    <col min="10" max="10" width="25" customWidth="1"/>
+    <col min="11" max="11" width="24.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="17.8571428571429" customWidth="1"/>
+    <col min="13" max="13" width="16.1428571428571" customWidth="1"/>
+    <col min="14" max="14" width="16.8571428571429" customWidth="1"/>
+    <col min="15" max="15" width="11.5714285714286" customWidth="1"/>
+    <col min="16" max="16" width="11.7142857142857" customWidth="1"/>
+    <col min="17" max="17" width="19.5714285714286" customWidth="1"/>
+    <col min="18" max="18" width="13.1428571428571" customWidth="1"/>
+    <col min="19" max="19" width="23.2857142857143" customWidth="1"/>
+    <col min="20" max="20" width="17" customWidth="1"/>
+    <col min="21" max="21" width="7.71428571428571" customWidth="1"/>
+    <col min="22" max="22" width="22.4285714285714" customWidth="1"/>
+    <col min="23" max="23" width="16.2857142857143" customWidth="1"/>
+    <col min="24" max="24" width="31.1428571428571" customWidth="1"/>
+    <col min="25" max="25" width="18.5714285714286" customWidth="1"/>
+    <col min="26" max="26" width="17.7142857142857" customWidth="1"/>
+    <col min="27" max="27" width="17.4285714285714" customWidth="1"/>
+    <col min="28" max="28" width="21.7142857142857" customWidth="1"/>
+    <col min="29" max="29" width="13.2857142857143" customWidth="1"/>
+    <col min="30" max="30" width="75" customWidth="1"/>
+    <col min="31" max="31" width="9.28571428571429" customWidth="1"/>
+    <col min="32" max="32" width="24.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="31.5" spans="1:31">
+    <row r="1" ht="31.5" spans="1:32">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1286,7 +1289,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1298,10 +1301,10 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="6" t="s">
@@ -1310,13 +1313,13 @@
       <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="8" t="s">
@@ -1334,7 +1337,7 @@
       <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="8" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="10" t="s">
@@ -1346,16 +1349,16 @@
       <c r="W1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="X1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Y1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="Z1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="15" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="2" t="s">
@@ -1370,162 +1373,171 @@
       <c r="AE1" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="AF1" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
-    <row r="2" ht="15.75" spans="1:31">
-      <c r="A2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" ht="15.75" spans="1:32">
+      <c r="A2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4">
+        <v>500</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4">
+      <c r="H2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="4"/>
+      <c r="J2" s="3">
         <v>1211</v>
       </c>
-      <c r="J2" s="5">
+      <c r="K2" s="4">
         <v>1211</v>
       </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5">
+      <c r="L2" s="9"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4">
         <v>10</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="13">
+        <v>5</v>
+      </c>
+      <c r="V2" s="14"/>
+      <c r="W2" s="13">
+        <v>0</v>
+      </c>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
+      <c r="AA2" s="14"/>
+      <c r="AB2" s="14"/>
+      <c r="AC2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF2" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" ht="15.75" spans="1:32">
+      <c r="A3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="4">
+        <v>100</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="I3" s="4"/>
+      <c r="J3" s="3">
+        <v>1211</v>
+      </c>
+      <c r="K3" s="4">
+        <v>1211</v>
+      </c>
+      <c r="L3" s="9"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4">
+        <v>30</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="Q3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="14">
+      <c r="S3" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="U3" s="13">
         <v>5</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="14">
+      <c r="V3" s="14"/>
+      <c r="W3" s="13">
         <v>0</v>
       </c>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="AC2" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="AD2" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE2" s="15" t="s">
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="AE3" s="14" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" spans="1:31">
-      <c r="A3" s="4" t="s">
+      <c r="AF3" s="14" t="s">
         <v>47</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="4">
-        <v>1211</v>
-      </c>
-      <c r="J3" s="5">
-        <v>1211</v>
-      </c>
-      <c r="K3" s="9"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5">
-        <v>30</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="T3" s="14">
-        <v>5</v>
-      </c>
-      <c r="U3" s="15"/>
-      <c r="V3" s="14">
-        <v>0</v>
-      </c>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC3" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD3" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="AE3" s="15" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE3">
+  <autoFilter ref="A1:AF3">
     <extLst/>
   </autoFilter>
-  <conditionalFormatting sqref="AC1:AC3">
+  <conditionalFormatting sqref="AD1:AD3">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>